<commit_message>
revisi excel for intructor review
</commit_message>
<xml_diff>
--- a/DataAlcohol.xlsx
+++ b/DataAlcohol.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william/Documents/Hacktiv8/p1/w4/alcoholadvisor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2139D213-F3B5-A34B-B5BA-EFEBDB3897D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695CB306-28C2-F846-A639-341F46D786C8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16340" xr2:uid="{58D54CBB-552C-5540-A91E-0925423FEB0E}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16340" activeTab="1" xr2:uid="{58D54CBB-552C-5540-A91E-0925423FEB0E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Informasi" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="74">
   <si>
     <t>isAlcohol</t>
   </si>
@@ -120,6 +121,138 @@
   </si>
   <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>MVP</t>
+  </si>
+  <si>
+    <t>Membangun sebuah platform yang membantu users untuk menentukan jenis minuman yang harus mereka pilih ketika mereka sedang berkunjung ke bar/lounge/club</t>
+  </si>
+  <si>
+    <t>Masalah User</t>
+  </si>
+  <si>
+    <t>Banyak orang yang masih asing dengan jenis minuman beralcohol yang disediakan oleh bar/lounge/club</t>
+  </si>
+  <si>
+    <t>Banyak orang yang memilih minuman berdasarkan promo yang sedang ada dan belum tentu cocok dengan selera</t>
+  </si>
+  <si>
+    <t>Banyak orang yang memilih minuman berdasarkan preferensi dari waiter/bartender</t>
+  </si>
+  <si>
+    <t>Solusi</t>
+  </si>
+  <si>
+    <t>Memberikan bantuan pilihan minuman berdasarkan selera users yang diinput ketika mereka registrasi</t>
+  </si>
+  <si>
+    <t>Memberikan opsi pilihan yang berbeda bila mereka memiliki perubahan selera</t>
+  </si>
+  <si>
+    <t>Memberikan mereka opsi untuk memilih secara manual minuman yang user suka</t>
+  </si>
+  <si>
+    <t>CRUD</t>
+  </si>
+  <si>
+    <t>Association Many to Many</t>
+  </si>
+  <si>
+    <t>Membuat hubungan antara userId dengan drinkId melalui conjunction table userdrink (many to many)</t>
+  </si>
+  <si>
+    <t>Association One to Many</t>
+  </si>
+  <si>
+    <t>Membuat hubungan antara drinkId dengan drinkCategoryId (one to many)</t>
+  </si>
+  <si>
+    <t>Helpers</t>
+  </si>
+  <si>
+    <t>Session and Encryption</t>
+  </si>
+  <si>
+    <t>Melakukan registrasi user baru dan password disimpan dalam bentuk encryption</t>
+  </si>
+  <si>
+    <t>Middleware</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Hooks</t>
+  </si>
+  <si>
+    <t>Sebelum registrasi berhasil dilakukan akan dilakukan pengecekan umur (beforeCreate - getAge)</t>
+  </si>
+  <si>
+    <t>Class/ Instance Method</t>
+  </si>
+  <si>
+    <t>Deploy to Heroku</t>
+  </si>
+  <si>
+    <t>Menampilkan registrasi awal</t>
+  </si>
+  <si>
+    <t>Melakukan validasi registrasi berdasarkan umur</t>
+  </si>
+  <si>
+    <t>Bila validasi berhasil, registrasi akan dilanjutkan halaman Profil User Attributes</t>
+  </si>
+  <si>
+    <t>Setelah seluruh User Attributes diisi, tampilkan halaman Rekomendasi Minuman</t>
+  </si>
+  <si>
+    <t>Membuat pilihan untuk melakukan update Rekomendasi Minuman</t>
+  </si>
+  <si>
+    <t>Opsi update 2: memilih minuman sendiri akan mengubah tampilan Rekomendasi Minuman</t>
+  </si>
+  <si>
+    <t>Opsi update 1: mengubah user attributes akan mengubah tampilan Rekomendasi Minuman</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Menghapus semua rekomendasi minuman</t>
+  </si>
+  <si>
+    <t>Menyimpan function getUserType (Beginner/Expert)</t>
+  </si>
+  <si>
+    <t>Menyimpan function getAge</t>
+  </si>
+  <si>
+    <t>Menampilkan halaman Homepage dengan Pilihan Semua Minuman di database (findAll Drink)</t>
+  </si>
+  <si>
+    <t>termasuk dalam pembuatan CRUD</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Partials</t>
+  </si>
+  <si>
+    <t>Membuat header dan disimpan dalam partial</t>
+  </si>
+  <si>
+    <t>Additional:</t>
   </si>
 </sst>
 </file>
@@ -143,15 +276,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -159,13 +298,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,7 +634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50DC7CA6-3CE6-2D4B-8B31-7DAB8FAC6D26}">
   <dimension ref="C5:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -817,4 +969,230 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14315CF0-E3E3-D040-BF23-E729ABF403C2}">
+  <dimension ref="B4:E35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="27.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="95.1640625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C11" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D27" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>